<commit_message>
Changed the AV rating curve code
streamline it to make better use of DataFrame and less of lists
</commit_message>
<xml_diff>
--- a/Data/Q/Fagaalu-StageDischarge.xlsx
+++ b/Data/Q/Fagaalu-StageDischarge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="405" windowWidth="19875" windowHeight="7695" tabRatio="762" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="480" yWindow="405" windowWidth="19875" windowHeight="7695" tabRatio="762" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -1443,6 +1443,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1548,11 +1549,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408122416"/>
-        <c:axId val="408120848"/>
+        <c:axId val="285821280"/>
+        <c:axId val="285821672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408122416"/>
+        <c:axId val="285821280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,18 +1575,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408120848"/>
+        <c:crossAx val="285821672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408120848"/>
+        <c:axId val="285821672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1608,13 +1610,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408122416"/>
+        <c:crossAx val="285821280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1778,11 +1781,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408124768"/>
-        <c:axId val="408125160"/>
+        <c:axId val="288464496"/>
+        <c:axId val="288465280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408124768"/>
+        <c:axId val="288464496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1792,7 +1795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408125160"/>
+        <c:crossAx val="288465280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1800,7 +1803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408125160"/>
+        <c:axId val="288465280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408124768"/>
+        <c:crossAx val="288464496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,11 +1978,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408130648"/>
-        <c:axId val="408131040"/>
+        <c:axId val="288466064"/>
+        <c:axId val="219651944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408130648"/>
+        <c:axId val="288466064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1992,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408131040"/>
+        <c:crossAx val="219651944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +2000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408131040"/>
+        <c:axId val="219651944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +2011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408130648"/>
+        <c:crossAx val="288466064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2172,11 +2175,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520071120"/>
-        <c:axId val="520071512"/>
+        <c:axId val="219655080"/>
+        <c:axId val="219653120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520071120"/>
+        <c:axId val="219655080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520071512"/>
+        <c:crossAx val="219653120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2194,7 +2197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520071512"/>
+        <c:axId val="219653120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520071120"/>
+        <c:crossAx val="219655080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2369,11 +2372,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520073472"/>
-        <c:axId val="520066808"/>
+        <c:axId val="219654296"/>
+        <c:axId val="219654688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520073472"/>
+        <c:axId val="219654296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520066808"/>
+        <c:crossAx val="219654688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2391,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520066808"/>
+        <c:axId val="219654688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520073472"/>
+        <c:crossAx val="219654296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2566,11 +2569,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520069552"/>
-        <c:axId val="520064064"/>
+        <c:axId val="305268464"/>
+        <c:axId val="305268856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520069552"/>
+        <c:axId val="305268464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520064064"/>
+        <c:crossAx val="305268856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2588,7 +2591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520064064"/>
+        <c:axId val="305268856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520069552"/>
+        <c:crossAx val="305268464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,11 +2766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520067200"/>
-        <c:axId val="520064456"/>
+        <c:axId val="305267288"/>
+        <c:axId val="366924392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520067200"/>
+        <c:axId val="305267288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,7 +2780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520064456"/>
+        <c:crossAx val="366924392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2785,7 +2788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520064456"/>
+        <c:axId val="366924392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2796,7 +2799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520067200"/>
+        <c:crossAx val="305267288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2960,11 +2963,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520069944"/>
-        <c:axId val="520067984"/>
+        <c:axId val="366925176"/>
+        <c:axId val="366925568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520069944"/>
+        <c:axId val="366925176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2974,7 +2977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520067984"/>
+        <c:crossAx val="366925568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2982,7 +2985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520067984"/>
+        <c:axId val="366925568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,7 +2996,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520069944"/>
+        <c:crossAx val="366925176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3157,11 +3160,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520068376"/>
-        <c:axId val="520072296"/>
+        <c:axId val="312189576"/>
+        <c:axId val="312189184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520068376"/>
+        <c:axId val="312189576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,7 +3174,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520072296"/>
+        <c:crossAx val="312189184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3179,7 +3182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520072296"/>
+        <c:axId val="312189184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3190,7 +3193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520068376"/>
+        <c:crossAx val="312189576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3402,11 +3405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520073864"/>
-        <c:axId val="520064848"/>
+        <c:axId val="312188792"/>
+        <c:axId val="312189968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520073864"/>
+        <c:axId val="312188792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3416,7 +3419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520064848"/>
+        <c:crossAx val="312189968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3424,7 +3427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520064848"/>
+        <c:axId val="312189968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,7 +3438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520073864"/>
+        <c:crossAx val="312188792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3599,11 +3602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520065240"/>
-        <c:axId val="520073080"/>
+        <c:axId val="312188008"/>
+        <c:axId val="312188400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520065240"/>
+        <c:axId val="312188008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,7 +3616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520073080"/>
+        <c:crossAx val="312188400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3621,7 +3624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520073080"/>
+        <c:axId val="312188400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3632,7 +3635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520065240"/>
+        <c:crossAx val="312188008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3870,11 +3873,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408126336"/>
-        <c:axId val="408121240"/>
+        <c:axId val="285822848"/>
+        <c:axId val="287561984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408126336"/>
+        <c:axId val="285822848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3894,12 +3897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408121240"/>
+        <c:crossAx val="287561984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408121240"/>
+        <c:axId val="287561984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3922,19 +3925,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408126336"/>
+        <c:crossAx val="285822848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4090,11 +4095,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520066024"/>
-        <c:axId val="520063280"/>
+        <c:axId val="312184480"/>
+        <c:axId val="312179384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520066024"/>
+        <c:axId val="312184480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4104,7 +4109,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520063280"/>
+        <c:crossAx val="312179384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4112,7 +4117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520063280"/>
+        <c:axId val="312179384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4123,7 +4128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520066024"/>
+        <c:crossAx val="312184480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4269,11 +4274,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520068768"/>
-        <c:axId val="520066416"/>
+        <c:axId val="312183696"/>
+        <c:axId val="312183304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520068768"/>
+        <c:axId val="312183696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4283,7 +4288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520066416"/>
+        <c:crossAx val="312183304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4291,7 +4296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520066416"/>
+        <c:axId val="312183304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,7 +4307,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520068768"/>
+        <c:crossAx val="312183696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4454,11 +4459,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520070336"/>
-        <c:axId val="520076608"/>
+        <c:axId val="312182520"/>
+        <c:axId val="312186048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520070336"/>
+        <c:axId val="312182520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4468,7 +4473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520076608"/>
+        <c:crossAx val="312186048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4476,7 +4481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520076608"/>
+        <c:axId val="312186048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4487,7 +4492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520070336"/>
+        <c:crossAx val="312182520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4644,11 +4649,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520075040"/>
-        <c:axId val="520074648"/>
+        <c:axId val="312184088"/>
+        <c:axId val="312185264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520075040"/>
+        <c:axId val="312184088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4658,7 +4663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520074648"/>
+        <c:crossAx val="312185264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4666,7 +4671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520074648"/>
+        <c:axId val="312185264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4677,7 +4682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520075040"/>
+        <c:crossAx val="312184088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4829,11 +4834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520077000"/>
-        <c:axId val="520077392"/>
+        <c:axId val="312185656"/>
+        <c:axId val="312187224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520077000"/>
+        <c:axId val="312185656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4843,7 +4848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520077392"/>
+        <c:crossAx val="312187224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4851,7 +4856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520077392"/>
+        <c:axId val="312187224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4862,7 +4867,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520077000"/>
+        <c:crossAx val="312185656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5014,11 +5019,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="520076216"/>
-        <c:axId val="412733320"/>
+        <c:axId val="312178600"/>
+        <c:axId val="312186440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="520076216"/>
+        <c:axId val="312178600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,7 +5033,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412733320"/>
+        <c:crossAx val="312186440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5036,7 +5041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412733320"/>
+        <c:axId val="312186440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5047,7 +5052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520076216"/>
+        <c:crossAx val="312178600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5204,11 +5209,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412733712"/>
-        <c:axId val="412734104"/>
+        <c:axId val="312179776"/>
+        <c:axId val="312177816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412733712"/>
+        <c:axId val="312179776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5218,7 +5223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412734104"/>
+        <c:crossAx val="312177816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5226,7 +5231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412734104"/>
+        <c:axId val="312177816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5237,7 +5242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412733712"/>
+        <c:crossAx val="312179776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5394,11 +5399,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412729792"/>
-        <c:axId val="412731752"/>
+        <c:axId val="312186832"/>
+        <c:axId val="312187616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412729792"/>
+        <c:axId val="312186832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5408,7 +5413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412731752"/>
+        <c:crossAx val="312187616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5416,7 +5421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412731752"/>
+        <c:axId val="312187616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5427,7 +5432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412729792"/>
+        <c:crossAx val="312186832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5590,11 +5595,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412734888"/>
-        <c:axId val="412731360"/>
+        <c:axId val="312180952"/>
+        <c:axId val="312175464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412734888"/>
+        <c:axId val="312180952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5604,7 +5609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412731360"/>
+        <c:crossAx val="312175464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5612,7 +5617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412731360"/>
+        <c:axId val="312175464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5623,7 +5628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412734888"/>
+        <c:crossAx val="312180952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5670,6 +5675,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5797,11 +5803,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412730184"/>
-        <c:axId val="412737632"/>
+        <c:axId val="312181344"/>
+        <c:axId val="312176640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412730184"/>
+        <c:axId val="312181344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5811,7 +5817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="412737632"/>
+        <c:crossAx val="312176640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5819,7 +5825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412737632"/>
+        <c:axId val="312176640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5830,13 +5836,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412730184"/>
+        <c:crossAx val="312181344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5969,11 +5976,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="408123200"/>
-        <c:axId val="408125944"/>
+        <c:axId val="287561592"/>
+        <c:axId val="287567472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408123200"/>
+        <c:axId val="287561592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5983,7 +5990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408125944"/>
+        <c:crossAx val="287567472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5991,7 +5998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408125944"/>
+        <c:axId val="287567472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6002,7 +6009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408123200"/>
+        <c:crossAx val="287561592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6174,11 +6181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412741552"/>
-        <c:axId val="412732144"/>
+        <c:axId val="312181736"/>
+        <c:axId val="312182128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412741552"/>
+        <c:axId val="312181736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6188,7 +6195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412732144"/>
+        <c:crossAx val="312182128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6196,7 +6203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412732144"/>
+        <c:axId val="312182128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6207,7 +6214,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412741552"/>
+        <c:crossAx val="312181736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6377,11 +6384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412740768"/>
-        <c:axId val="412730576"/>
+        <c:axId val="368397064"/>
+        <c:axId val="368406472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412740768"/>
+        <c:axId val="368397064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6391,7 +6398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412730576"/>
+        <c:crossAx val="368406472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6399,7 +6406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412730576"/>
+        <c:axId val="368406472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6410,7 +6417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412740768"/>
+        <c:crossAx val="368397064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6580,11 +6587,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412732928"/>
-        <c:axId val="412735280"/>
+        <c:axId val="368395888"/>
+        <c:axId val="368400984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412732928"/>
+        <c:axId val="368395888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6594,7 +6601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412735280"/>
+        <c:crossAx val="368400984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6602,7 +6609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412735280"/>
+        <c:axId val="368400984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6613,7 +6620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412732928"/>
+        <c:crossAx val="368395888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6777,11 +6784,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412737240"/>
-        <c:axId val="412735672"/>
+        <c:axId val="368405296"/>
+        <c:axId val="368399416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412737240"/>
+        <c:axId val="368405296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6791,7 +6798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412735672"/>
+        <c:crossAx val="368399416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6799,7 +6806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412735672"/>
+        <c:axId val="368399416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6810,7 +6817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412737240"/>
+        <c:crossAx val="368405296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6980,11 +6987,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412736456"/>
-        <c:axId val="412736848"/>
+        <c:axId val="368398240"/>
+        <c:axId val="368403728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412736456"/>
+        <c:axId val="368398240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6994,7 +7001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412736848"/>
+        <c:crossAx val="368403728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7002,7 +7009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412736848"/>
+        <c:axId val="368403728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7013,7 +7020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412736456"/>
+        <c:crossAx val="368398240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7177,11 +7184,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412738416"/>
-        <c:axId val="412739984"/>
+        <c:axId val="368402552"/>
+        <c:axId val="368397456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412738416"/>
+        <c:axId val="368402552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7191,7 +7198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412739984"/>
+        <c:crossAx val="368397456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7199,7 +7206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412739984"/>
+        <c:axId val="368397456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7210,7 +7217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412738416"/>
+        <c:crossAx val="368402552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7380,11 +7387,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412752920"/>
-        <c:axId val="412746648"/>
+        <c:axId val="368394712"/>
+        <c:axId val="368399808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412752920"/>
+        <c:axId val="368394712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7394,7 +7401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412746648"/>
+        <c:crossAx val="368399808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7402,7 +7409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412746648"/>
+        <c:axId val="368399808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7413,7 +7420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412752920"/>
+        <c:crossAx val="368394712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7577,11 +7584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412743120"/>
-        <c:axId val="412743512"/>
+        <c:axId val="368399024"/>
+        <c:axId val="368400200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412743120"/>
+        <c:axId val="368399024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7591,7 +7598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412743512"/>
+        <c:crossAx val="368400200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7599,7 +7606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412743512"/>
+        <c:axId val="368400200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7610,7 +7617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412743120"/>
+        <c:crossAx val="368399024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7780,11 +7787,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412745080"/>
-        <c:axId val="412750176"/>
+        <c:axId val="368404120"/>
+        <c:axId val="368395104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412745080"/>
+        <c:axId val="368404120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7794,7 +7801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412750176"/>
+        <c:crossAx val="368395104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7802,7 +7809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412750176"/>
+        <c:axId val="368395104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7813,7 +7820,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412745080"/>
+        <c:crossAx val="368404120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7977,11 +7984,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412744688"/>
-        <c:axId val="412747040"/>
+        <c:axId val="368401768"/>
+        <c:axId val="368402160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412744688"/>
+        <c:axId val="368401768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7991,7 +7998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412747040"/>
+        <c:crossAx val="368402160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7999,7 +8006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412747040"/>
+        <c:axId val="368402160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8010,7 +8017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412744688"/>
+        <c:crossAx val="368401768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8057,6 +8064,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8165,11 +8173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408125552"/>
-        <c:axId val="408127904"/>
+        <c:axId val="287563552"/>
+        <c:axId val="287568256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408125552"/>
+        <c:axId val="287563552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8191,18 +8199,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408127904"/>
+        <c:crossAx val="287568256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408127904"/>
+        <c:axId val="287568256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8225,13 +8234,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408125552"/>
+        <c:crossAx val="287563552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8401,11 +8411,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412754096"/>
-        <c:axId val="412752528"/>
+        <c:axId val="368403336"/>
+        <c:axId val="368404904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412754096"/>
+        <c:axId val="368403336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8415,7 +8425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412752528"/>
+        <c:crossAx val="368404904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8423,7 +8433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412752528"/>
+        <c:axId val="368404904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8434,7 +8444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412754096"/>
+        <c:crossAx val="368403336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8598,11 +8608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412749000"/>
-        <c:axId val="412742336"/>
+        <c:axId val="368405688"/>
+        <c:axId val="368406080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412749000"/>
+        <c:axId val="368405688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8612,7 +8622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412742336"/>
+        <c:crossAx val="368406080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8620,7 +8630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412742336"/>
+        <c:axId val="368406080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8631,7 +8641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412749000"/>
+        <c:crossAx val="368405688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8801,11 +8811,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412751744"/>
-        <c:axId val="412743904"/>
+        <c:axId val="368411960"/>
+        <c:axId val="368411568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412751744"/>
+        <c:axId val="368411960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8815,7 +8825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412743904"/>
+        <c:crossAx val="368411568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8823,7 +8833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412743904"/>
+        <c:axId val="368411568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8834,7 +8844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412751744"/>
+        <c:crossAx val="368411960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8998,11 +9008,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412748216"/>
-        <c:axId val="412753312"/>
+        <c:axId val="368406864"/>
+        <c:axId val="368409608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412748216"/>
+        <c:axId val="368406864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9012,7 +9022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412753312"/>
+        <c:crossAx val="368409608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9020,7 +9030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412753312"/>
+        <c:axId val="368409608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9031,7 +9041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412748216"/>
+        <c:crossAx val="368406864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9201,11 +9211,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412744296"/>
-        <c:axId val="412745472"/>
+        <c:axId val="368408040"/>
+        <c:axId val="368412744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412744296"/>
+        <c:axId val="368408040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9215,7 +9225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412745472"/>
+        <c:crossAx val="368412744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9223,7 +9233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412745472"/>
+        <c:axId val="368412744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9234,7 +9244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412744296"/>
+        <c:crossAx val="368408040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9398,11 +9408,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412748608"/>
-        <c:axId val="412752136"/>
+        <c:axId val="368408824"/>
+        <c:axId val="368410392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412748608"/>
+        <c:axId val="368408824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9412,7 +9422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412752136"/>
+        <c:crossAx val="368410392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9420,7 +9430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412752136"/>
+        <c:axId val="368410392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9431,7 +9441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412748608"/>
+        <c:crossAx val="368408824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9601,11 +9611,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412750568"/>
-        <c:axId val="412749784"/>
+        <c:axId val="368407256"/>
+        <c:axId val="368413528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412750568"/>
+        <c:axId val="368407256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9615,7 +9625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412749784"/>
+        <c:crossAx val="368413528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9623,7 +9633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412749784"/>
+        <c:axId val="368413528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9634,7 +9644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412750568"/>
+        <c:crossAx val="368407256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9798,11 +9808,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412760760"/>
-        <c:axId val="412758408"/>
+        <c:axId val="368413136"/>
+        <c:axId val="368407648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412760760"/>
+        <c:axId val="368413136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9812,7 +9822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412758408"/>
+        <c:crossAx val="368407648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9820,7 +9830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412758408"/>
+        <c:axId val="368407648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9831,7 +9841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412760760"/>
+        <c:crossAx val="368413136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10001,11 +10011,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412761544"/>
-        <c:axId val="412754880"/>
+        <c:axId val="368391184"/>
+        <c:axId val="368384520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412761544"/>
+        <c:axId val="368391184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10015,7 +10025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412754880"/>
+        <c:crossAx val="368384520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10023,7 +10033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412754880"/>
+        <c:axId val="368384520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10034,7 +10044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412761544"/>
+        <c:crossAx val="368391184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10198,11 +10208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412754488"/>
-        <c:axId val="412755272"/>
+        <c:axId val="368388048"/>
+        <c:axId val="368382168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412754488"/>
+        <c:axId val="368388048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10212,7 +10222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412755272"/>
+        <c:crossAx val="368382168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10220,7 +10230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412755272"/>
+        <c:axId val="368382168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10231,7 +10241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412754488"/>
+        <c:crossAx val="368388048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10286,6 +10296,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10329,19 +10340,19 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$C$36:$C$47</c:f>
+              <c:f>Summary!$C$36:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$D$36:$D$47</c:f>
+              <c:f>Summary!$D$36:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.5303373000000002E-2</c:v>
                 </c:pt>
@@ -10349,33 +10360,27 @@
                   <c:v>0.18668238000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5303373000000002E-2</c:v>
+                  <c:v>0.18544031999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18668238000000001</c:v>
+                  <c:v>0.23222712000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18544031999999999</c:v>
+                  <c:v>0.24001475999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23222712000000006</c:v>
+                  <c:v>0.17199864000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24001475999999999</c:v>
+                  <c:v>0.22887431999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17199864000000001</c:v>
+                  <c:v>0.23029164000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.22887431999999999</c:v>
+                  <c:v>0.23173943999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23029164000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.23173943999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.22485096000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -10391,11 +10396,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408128688"/>
-        <c:axId val="408118888"/>
+        <c:axId val="287564728"/>
+        <c:axId val="287565512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408128688"/>
+        <c:axId val="287564728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10417,18 +10422,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408118888"/>
+        <c:crossAx val="287565512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408118888"/>
+        <c:axId val="287565512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10451,13 +10457,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408128688"/>
+        <c:crossAx val="287564728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10621,11 +10628,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412756448"/>
-        <c:axId val="412756840"/>
+        <c:axId val="368390792"/>
+        <c:axId val="368393928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412756448"/>
+        <c:axId val="368390792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10635,7 +10642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412756840"/>
+        <c:crossAx val="368393928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10643,7 +10650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412756840"/>
+        <c:axId val="368393928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10654,7 +10661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412756448"/>
+        <c:crossAx val="368390792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10818,11 +10825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412758800"/>
-        <c:axId val="412760368"/>
+        <c:axId val="368383344"/>
+        <c:axId val="368381776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412758800"/>
+        <c:axId val="368383344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10832,7 +10839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412760368"/>
+        <c:crossAx val="368381776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10840,7 +10847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412760368"/>
+        <c:axId val="368381776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10851,7 +10858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412758800"/>
+        <c:crossAx val="368383344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11015,11 +11022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412756056"/>
-        <c:axId val="412759192"/>
+        <c:axId val="368389616"/>
+        <c:axId val="368387264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412756056"/>
+        <c:axId val="368389616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11029,7 +11036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412759192"/>
+        <c:crossAx val="368387264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11037,7 +11044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412759192"/>
+        <c:axId val="368387264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11048,7 +11055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412756056"/>
+        <c:crossAx val="368389616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11212,11 +11219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496852520"/>
-        <c:axId val="496851344"/>
+        <c:axId val="368384128"/>
+        <c:axId val="368386480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496852520"/>
+        <c:axId val="368384128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11226,7 +11233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496851344"/>
+        <c:crossAx val="368386480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11234,7 +11241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496851344"/>
+        <c:axId val="368386480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11245,7 +11252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496852520"/>
+        <c:crossAx val="368384128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11403,11 +11410,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496843504"/>
-        <c:axId val="496840760"/>
+        <c:axId val="368385696"/>
+        <c:axId val="368391968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496843504"/>
+        <c:axId val="368385696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11417,7 +11424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496840760"/>
+        <c:crossAx val="368391968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11425,7 +11432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496840760"/>
+        <c:axId val="368391968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11436,7 +11443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496843504"/>
+        <c:crossAx val="368385696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11582,11 +11589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496847032"/>
-        <c:axId val="496849384"/>
+        <c:axId val="368384912"/>
+        <c:axId val="368385304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496847032"/>
+        <c:axId val="368384912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11596,7 +11603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496849384"/>
+        <c:crossAx val="368385304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11604,7 +11611,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496849384"/>
+        <c:axId val="368385304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11615,7 +11622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496847032"/>
+        <c:crossAx val="368384912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11767,11 +11774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496843896"/>
-        <c:axId val="496845072"/>
+        <c:axId val="368386088"/>
+        <c:axId val="368393144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496843896"/>
+        <c:axId val="368386088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11781,7 +11788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496845072"/>
+        <c:crossAx val="368393144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11789,7 +11796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496845072"/>
+        <c:axId val="368393144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11800,7 +11807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496843896"/>
+        <c:crossAx val="368386088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11958,11 +11965,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496841152"/>
-        <c:axId val="496845856"/>
+        <c:axId val="368387656"/>
+        <c:axId val="368388440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496841152"/>
+        <c:axId val="368387656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11972,7 +11979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496845856"/>
+        <c:crossAx val="368388440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11980,7 +11987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496845856"/>
+        <c:axId val="368388440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11991,7 +11998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496841152"/>
+        <c:crossAx val="368387656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12280,11 +12287,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="496841544"/>
-        <c:axId val="496844680"/>
+        <c:axId val="368389224"/>
+        <c:axId val="368390008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="496841544"/>
+        <c:axId val="368389224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12344,12 +12351,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496844680"/>
+        <c:crossAx val="368390008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="496844680"/>
+        <c:axId val="368390008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12408,7 +12415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496841544"/>
+        <c:crossAx val="368389224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12562,8 +12569,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="496841936"/>
-        <c:axId val="496847424"/>
+        <c:axId val="371665568"/>
+        <c:axId val="371658120"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12717,11 +12724,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="496841936"/>
-        <c:axId val="496847424"/>
+        <c:axId val="371665568"/>
+        <c:axId val="371658120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496841936"/>
+        <c:axId val="371665568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12731,7 +12738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496847424"/>
+        <c:crossAx val="371658120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12739,7 +12746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496847424"/>
+        <c:axId val="371658120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12750,7 +12757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496841936"/>
+        <c:crossAx val="371665568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12952,11 +12959,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408129080"/>
-        <c:axId val="408129472"/>
+        <c:axId val="305234808"/>
+        <c:axId val="305235200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408129080"/>
+        <c:axId val="305234808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12966,7 +12973,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408129472"/>
+        <c:crossAx val="305235200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12974,7 +12981,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408129472"/>
+        <c:axId val="305235200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12985,7 +12992,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408129080"/>
+        <c:crossAx val="305234808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13089,8 +13096,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="496846248"/>
-        <c:axId val="496847816"/>
+        <c:axId val="371654984"/>
+        <c:axId val="371660472"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13208,11 +13215,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="496846248"/>
-        <c:axId val="496847816"/>
+        <c:axId val="371654984"/>
+        <c:axId val="371660472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496846248"/>
+        <c:axId val="371654984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13222,7 +13229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496847816"/>
+        <c:crossAx val="371660472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13230,7 +13237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496847816"/>
+        <c:axId val="371660472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13241,7 +13248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="496846248"/>
+        <c:crossAx val="371654984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13409,11 +13416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408131824"/>
-        <c:axId val="408132216"/>
+        <c:axId val="305232848"/>
+        <c:axId val="305231280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408131824"/>
+        <c:axId val="305232848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13423,7 +13430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408132216"/>
+        <c:crossAx val="305231280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13431,7 +13438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408132216"/>
+        <c:axId val="305231280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13442,7 +13449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408131824"/>
+        <c:crossAx val="305232848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13606,11 +13613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408132608"/>
-        <c:axId val="408133000"/>
+        <c:axId val="305233632"/>
+        <c:axId val="305234416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408132608"/>
+        <c:axId val="305233632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13620,7 +13627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408133000"/>
+        <c:crossAx val="305234416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13628,7 +13635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408133000"/>
+        <c:axId val="305234416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13639,7 +13646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408132608"/>
+        <c:crossAx val="305233632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13803,11 +13810,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="408128296"/>
-        <c:axId val="408119280"/>
+        <c:axId val="288462928"/>
+        <c:axId val="288463320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="408128296"/>
+        <c:axId val="288462928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13817,7 +13824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408119280"/>
+        <c:crossAx val="288463320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13825,7 +13832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408119280"/>
+        <c:axId val="288463320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13836,7 +13843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408128296"/>
+        <c:crossAx val="288462928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14541,7 +14548,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16651,10 +16658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17115,30 +17122,30 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>40919</v>
+        <v>40933</v>
       </c>
       <c r="B38">
-        <v>1200</v>
+        <v>938</v>
       </c>
       <c r="D38">
-        <v>1.5303373000000002E-2</v>
+        <v>0.18544031999999999</v>
       </c>
       <c r="E38">
-        <v>15.303373000000002</v>
+        <v>185.44031999999999</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>40927</v>
+        <v>40933</v>
       </c>
       <c r="B39">
-        <v>1449</v>
+        <v>1000</v>
       </c>
       <c r="D39">
-        <v>0.18668238000000001</v>
+        <v>0.23222712000000006</v>
       </c>
       <c r="E39">
-        <v>186.68237999999999</v>
+        <v>232.22712000000007</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -17146,13 +17153,13 @@
         <v>40933</v>
       </c>
       <c r="B40">
-        <v>938</v>
+        <v>1015</v>
       </c>
       <c r="D40">
-        <v>0.18544031999999999</v>
+        <v>0.24001475999999999</v>
       </c>
       <c r="E40">
-        <v>185.44031999999999</v>
+        <v>240.01476</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -17160,13 +17167,13 @@
         <v>40933</v>
       </c>
       <c r="B41">
-        <v>1000</v>
+        <v>1115</v>
       </c>
       <c r="D41">
-        <v>0.23222712000000006</v>
+        <v>0.17199864000000001</v>
       </c>
       <c r="E41">
-        <v>232.22712000000007</v>
+        <v>171.99863999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -17174,13 +17181,13 @@
         <v>40933</v>
       </c>
       <c r="B42">
-        <v>1015</v>
+        <v>1125</v>
       </c>
       <c r="D42">
-        <v>0.24001475999999999</v>
+        <v>0.22887431999999999</v>
       </c>
       <c r="E42">
-        <v>240.01476</v>
+        <v>228.87431999999998</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17188,13 +17195,13 @@
         <v>40933</v>
       </c>
       <c r="B43">
-        <v>1115</v>
+        <v>1129</v>
       </c>
       <c r="D43">
-        <v>0.17199864000000001</v>
+        <v>0.23029164000000002</v>
       </c>
       <c r="E43">
-        <v>171.99863999999999</v>
+        <v>230.29164000000003</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -17202,13 +17209,13 @@
         <v>40933</v>
       </c>
       <c r="B44">
-        <v>1125</v>
+        <v>1145</v>
       </c>
       <c r="D44">
-        <v>0.22887431999999999</v>
+        <v>0.23173943999999999</v>
       </c>
       <c r="E44">
-        <v>228.87431999999998</v>
+        <v>231.73944</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -17216,40 +17223,12 @@
         <v>40933</v>
       </c>
       <c r="B45">
-        <v>1129</v>
+        <v>1200</v>
       </c>
       <c r="D45">
-        <v>0.23029164000000002</v>
+        <v>0.22485096000000002</v>
       </c>
       <c r="E45">
-        <v>230.29164000000003</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>40933</v>
-      </c>
-      <c r="B46">
-        <v>1145</v>
-      </c>
-      <c r="D46">
-        <v>0.23173943999999999</v>
-      </c>
-      <c r="E46">
-        <v>231.73944</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>40933</v>
-      </c>
-      <c r="B47">
-        <v>1200</v>
-      </c>
-      <c r="D47">
-        <v>0.22485096000000002</v>
-      </c>
-      <c r="E47">
         <v>224.85096000000001</v>
       </c>
     </row>
@@ -19023,7 +19002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -20259,11 +20238,11 @@
         <v>41387</v>
       </c>
       <c r="D21" s="56">
-        <f t="shared" ref="D21:D24" si="25">D20</f>
+        <f t="shared" ref="D21:D23" si="25">D20</f>
         <v>1535</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" ref="E21:E24" si="26">E20</f>
+        <f t="shared" ref="E21:E23" si="26">E20</f>
         <v>93</v>
       </c>
       <c r="F21" s="150">
@@ -20633,11 +20612,11 @@
         <v>41387</v>
       </c>
       <c r="D27" s="56">
-        <f t="shared" ref="D27:D28" si="34">D26</f>
+        <f t="shared" ref="D27" si="34">D26</f>
         <v>1630</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" ref="E27:E28" si="35">E26</f>
+        <f t="shared" ref="E27" si="35">E26</f>
         <v>69</v>
       </c>
       <c r="F27" s="150">
@@ -20654,7 +20633,7 @@
         <v>61</v>
       </c>
       <c r="J27" s="58">
-        <f t="shared" ref="J27:J34" si="36">I27/2.54/12</f>
+        <f t="shared" ref="J27:J33" si="36">I27/2.54/12</f>
         <v>2.0013123359580054</v>
       </c>
       <c r="K27" s="57">
@@ -21269,47 +21248,47 @@
         <v>40</v>
       </c>
       <c r="F37" s="151">
-        <f>AVERAGE(F35:F36)</f>
+        <f t="shared" ref="F37:P37" si="73">AVERAGE(F35:F36)</f>
         <v>16.5</v>
       </c>
       <c r="G37" s="28">
-        <f>AVERAGE(G35:G36)</f>
+        <f t="shared" si="73"/>
         <v>16.5</v>
       </c>
       <c r="H37" s="144">
-        <f>AVERAGE(H35:H36)</f>
+        <f t="shared" si="73"/>
         <v>1.3123359580052494</v>
       </c>
       <c r="I37" s="144">
-        <f>AVERAGE(I35:I36)</f>
+        <f t="shared" si="73"/>
         <v>37.200000000000003</v>
       </c>
       <c r="J37" s="60">
-        <f>AVERAGE(J35:J36)</f>
+        <f t="shared" si="73"/>
         <v>1.2204724409448819</v>
       </c>
       <c r="K37" s="144">
-        <f>AVERAGE(K35:K36)</f>
+        <f t="shared" si="73"/>
         <v>20.137795275590552</v>
       </c>
       <c r="L37" s="60">
-        <f>AVERAGE(L35:L36)</f>
+        <f t="shared" si="73"/>
         <v>6.3461538461538467</v>
       </c>
       <c r="M37" s="60">
-        <f>AVERAGE(M35:M36)</f>
+        <f t="shared" si="73"/>
         <v>1.9343076923076925</v>
       </c>
       <c r="N37" s="60">
-        <f>AVERAGE(N35:N36)</f>
+        <f t="shared" si="73"/>
         <v>2.8</v>
       </c>
       <c r="O37" s="144">
-        <f>AVERAGE(O35:O36)</f>
+        <f t="shared" si="73"/>
         <v>357.83313143549367</v>
       </c>
       <c r="P37" s="59">
-        <f>AVERAGE(P35:P36)</f>
+        <f t="shared" si="73"/>
         <v>10132.70588875168</v>
       </c>
       <c r="Q37" s="135">
@@ -21344,7 +21323,7 @@
         <v>16.5</v>
       </c>
       <c r="H38" s="71">
-        <f t="shared" ref="H38" si="73">E38/2.54/12</f>
+        <f t="shared" ref="H38" si="74">E38/2.54/12</f>
         <v>1.0498687664041995</v>
       </c>
       <c r="I38" s="145">
@@ -21355,26 +21334,26 @@
         <v>0.90223097112860895</v>
       </c>
       <c r="K38" s="145">
-        <f t="shared" ref="K38" si="74">G38*J38</f>
+        <f t="shared" ref="K38" si="75">G38*J38</f>
         <v>14.886811023622048</v>
       </c>
       <c r="L38" s="146">
-        <f t="shared" ref="L38" si="75">100/F38</f>
+        <f t="shared" ref="L38" si="76">100/F38</f>
         <v>5.882352941176471</v>
       </c>
       <c r="M38" s="146">
-        <f t="shared" ref="M38" si="76">L38*0.3048</f>
+        <f t="shared" ref="M38" si="77">L38*0.3048</f>
         <v>1.7929411764705885</v>
       </c>
       <c r="N38" s="72">
         <v>2.8</v>
       </c>
       <c r="O38" s="71">
-        <f t="shared" ref="O38" si="77">L38*N38*K38</f>
+        <f t="shared" ref="O38" si="78">L38*N38*K38</f>
         <v>245.19453450671611</v>
       </c>
       <c r="P38" s="74">
-        <f t="shared" ref="P38" si="78">O38*28.316846593</f>
+        <f t="shared" ref="P38" si="79">O38*28.316846593</f>
         <v>6943.1360190687255</v>
       </c>
       <c r="Q38" s="74">
@@ -40727,8 +40706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T331"/>
   <sheetViews>
-    <sheetView topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="B317" sqref="B317:J331"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mannings for DAM and LBJ
Worked on calibrating Mannings n for both
</commit_message>
<xml_diff>
--- a/Data/Q/Fagaalu-StageDischarge.xlsx
+++ b/Data/Q/Fagaalu-StageDischarge.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="405" windowWidth="19875" windowHeight="7695" tabRatio="762" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="405" windowWidth="19875" windowHeight="7695" tabRatio="762" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
     <sheet name="LBJ" sheetId="1" r:id="rId2"/>
     <sheet name="DT" sheetId="2" r:id="rId3"/>
     <sheet name="Dam" sheetId="3" r:id="rId4"/>
-    <sheet name="Float" sheetId="13" r:id="rId5"/>
-    <sheet name="LBJ-1_19a" sheetId="8" r:id="rId6"/>
-    <sheet name="LBJ-1_19b" sheetId="9" r:id="rId7"/>
-    <sheet name="LBJ-1_19c" sheetId="4" r:id="rId8"/>
-    <sheet name="DT-1_13" sheetId="6" r:id="rId9"/>
-    <sheet name="DT-1_19a" sheetId="7" r:id="rId10"/>
-    <sheet name="DT-1_19b" sheetId="11" r:id="rId11"/>
-    <sheet name="DT-1_19c" sheetId="12" r:id="rId12"/>
-    <sheet name="Dam-1_19" sheetId="10" r:id="rId13"/>
-    <sheet name="OrangePeel" sheetId="14" r:id="rId14"/>
-    <sheet name="FieldFormFloat" sheetId="18" r:id="rId15"/>
-    <sheet name="FieldFormAV" sheetId="17" r:id="rId16"/>
-    <sheet name="Rectangular binsLBJ" sheetId="15" r:id="rId17"/>
-    <sheet name="Rectangular binsDAM" sheetId="16" r:id="rId18"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId5"/>
+    <sheet name="Float" sheetId="13" r:id="rId6"/>
+    <sheet name="LBJ-1_19a" sheetId="8" r:id="rId7"/>
+    <sheet name="LBJ-1_19b" sheetId="9" r:id="rId8"/>
+    <sheet name="LBJ-1_19c" sheetId="4" r:id="rId9"/>
+    <sheet name="DT-1_13" sheetId="6" r:id="rId10"/>
+    <sheet name="DT-1_19a" sheetId="7" r:id="rId11"/>
+    <sheet name="DT-1_19b" sheetId="11" r:id="rId12"/>
+    <sheet name="DT-1_19c" sheetId="12" r:id="rId13"/>
+    <sheet name="Dam-1_19" sheetId="10" r:id="rId14"/>
+    <sheet name="OrangePeel" sheetId="14" r:id="rId15"/>
+    <sheet name="FieldFormFloat" sheetId="18" r:id="rId16"/>
+    <sheet name="FieldFormAV" sheetId="17" r:id="rId17"/>
+    <sheet name="Rectangular binsLBJ" sheetId="15" r:id="rId18"/>
+    <sheet name="Rectangular binsDAM" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1548,11 +1549,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="281197528"/>
-        <c:axId val="281190472"/>
+        <c:axId val="319690952"/>
+        <c:axId val="319698400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="281197528"/>
+        <c:axId val="319690952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,12 +1581,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="281190472"/>
+        <c:crossAx val="319698400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281190472"/>
+        <c:axId val="319698400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,7 +1615,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="281197528"/>
+        <c:crossAx val="319690952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1778,11 +1779,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296257488"/>
-        <c:axId val="296262584"/>
+        <c:axId val="331117344"/>
+        <c:axId val="331113032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296257488"/>
+        <c:axId val="331117344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1792,7 +1793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296262584"/>
+        <c:crossAx val="331113032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1800,7 +1801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296262584"/>
+        <c:axId val="331113032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296257488"/>
+        <c:crossAx val="331117344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296261408"/>
-        <c:axId val="296256312"/>
+        <c:axId val="331113424"/>
+        <c:axId val="331114600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296261408"/>
+        <c:axId val="331113424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296256312"/>
+        <c:crossAx val="331114600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +1998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296256312"/>
+        <c:axId val="331114600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +2009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296261408"/>
+        <c:crossAx val="331113424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2172,11 +2173,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296257096"/>
-        <c:axId val="296257880"/>
+        <c:axId val="331098136"/>
+        <c:axId val="218633488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296257096"/>
+        <c:axId val="331098136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296257880"/>
+        <c:crossAx val="218633488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2194,7 +2195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296257880"/>
+        <c:axId val="218633488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296257096"/>
+        <c:crossAx val="331098136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2369,11 +2370,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296258272"/>
-        <c:axId val="283656800"/>
+        <c:axId val="218638192"/>
+        <c:axId val="218639760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296258272"/>
+        <c:axId val="218638192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283656800"/>
+        <c:crossAx val="218639760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2391,7 +2392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283656800"/>
+        <c:axId val="218639760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296258272"/>
+        <c:crossAx val="218638192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2566,11 +2567,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="283657976"/>
-        <c:axId val="283659936"/>
+        <c:axId val="218634272"/>
+        <c:axId val="218638584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="283657976"/>
+        <c:axId val="218634272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283659936"/>
+        <c:crossAx val="218638584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2588,7 +2589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283659936"/>
+        <c:axId val="218638584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283657976"/>
+        <c:crossAx val="218634272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,11 +2764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296804976"/>
-        <c:axId val="296805368"/>
+        <c:axId val="218638976"/>
+        <c:axId val="218640936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296804976"/>
+        <c:axId val="218638976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,7 +2778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296805368"/>
+        <c:crossAx val="218640936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2785,7 +2786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296805368"/>
+        <c:axId val="218640936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2796,7 +2797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296804976"/>
+        <c:crossAx val="218638976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2960,11 +2961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296810072"/>
-        <c:axId val="296808112"/>
+        <c:axId val="218634664"/>
+        <c:axId val="218637016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296810072"/>
+        <c:axId val="218634664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2974,7 +2975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296808112"/>
+        <c:crossAx val="218637016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2982,7 +2983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296808112"/>
+        <c:axId val="218637016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,7 +2994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296810072"/>
+        <c:crossAx val="218634664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3157,11 +3158,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296811640"/>
-        <c:axId val="296806544"/>
+        <c:axId val="218635448"/>
+        <c:axId val="218635840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296811640"/>
+        <c:axId val="218635448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,7 +3172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296806544"/>
+        <c:crossAx val="218635840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3179,7 +3180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296806544"/>
+        <c:axId val="218635840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3190,7 +3191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296811640"/>
+        <c:crossAx val="218635448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3402,11 +3403,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296804584"/>
-        <c:axId val="296805760"/>
+        <c:axId val="218636624"/>
+        <c:axId val="218637408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296804584"/>
+        <c:axId val="218636624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3416,7 +3417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296805760"/>
+        <c:crossAx val="218637408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3424,7 +3425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296805760"/>
+        <c:axId val="218637408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,7 +3436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296804584"/>
+        <c:crossAx val="218636624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3599,11 +3600,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296810856"/>
-        <c:axId val="296806152"/>
+        <c:axId val="316204208"/>
+        <c:axId val="316205384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296810856"/>
+        <c:axId val="316204208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,7 +3614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296806152"/>
+        <c:crossAx val="316205384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3621,7 +3622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296806152"/>
+        <c:axId val="316205384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3632,7 +3633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296810856"/>
+        <c:crossAx val="316204208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3870,11 +3871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="283661896"/>
-        <c:axId val="283658760"/>
+        <c:axId val="319691344"/>
+        <c:axId val="319696048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="283661896"/>
+        <c:axId val="319691344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3894,12 +3895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283658760"/>
+        <c:crossAx val="319696048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="283658760"/>
+        <c:axId val="319696048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3928,7 +3929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283661896"/>
+        <c:crossAx val="319691344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4090,11 +4091,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296808504"/>
-        <c:axId val="296808896"/>
+        <c:axId val="316206560"/>
+        <c:axId val="261381880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296808504"/>
+        <c:axId val="316206560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4104,7 +4105,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296808896"/>
+        <c:crossAx val="261381880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4112,7 +4113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296808896"/>
+        <c:axId val="261381880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4123,7 +4124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296808504"/>
+        <c:crossAx val="316206560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4269,11 +4270,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296810464"/>
-        <c:axId val="296811248"/>
+        <c:axId val="261383056"/>
+        <c:axId val="318110224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296810464"/>
+        <c:axId val="261383056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4283,7 +4284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296811248"/>
+        <c:crossAx val="318110224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4291,7 +4292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296811248"/>
+        <c:axId val="318110224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,7 +4303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296810464"/>
+        <c:crossAx val="261383056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4454,11 +4455,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296151232"/>
-        <c:axId val="296147704"/>
+        <c:axId val="418609616"/>
+        <c:axId val="431731752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296151232"/>
+        <c:axId val="418609616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4468,7 +4469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296147704"/>
+        <c:crossAx val="431731752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4476,7 +4477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296147704"/>
+        <c:axId val="431731752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4487,7 +4488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296151232"/>
+        <c:crossAx val="418609616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4644,11 +4645,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296151624"/>
-        <c:axId val="296148096"/>
+        <c:axId val="431737240"/>
+        <c:axId val="431732928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296151624"/>
+        <c:axId val="431737240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4658,7 +4659,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296148096"/>
+        <c:crossAx val="431732928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4666,7 +4667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296148096"/>
+        <c:axId val="431732928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4677,7 +4678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296151624"/>
+        <c:crossAx val="431737240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4829,11 +4830,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296152016"/>
-        <c:axId val="296150448"/>
+        <c:axId val="431732144"/>
+        <c:axId val="431733320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296152016"/>
+        <c:axId val="431732144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4843,7 +4844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296150448"/>
+        <c:crossAx val="431733320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4851,7 +4852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296150448"/>
+        <c:axId val="431733320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4862,7 +4863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296152016"/>
+        <c:crossAx val="431732144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5014,11 +5015,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296152408"/>
-        <c:axId val="296152800"/>
+        <c:axId val="431733712"/>
+        <c:axId val="431734104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296152408"/>
+        <c:axId val="431733712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,7 +5029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296152800"/>
+        <c:crossAx val="431734104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5036,7 +5037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296152800"/>
+        <c:axId val="431734104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5047,7 +5048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296152408"/>
+        <c:crossAx val="431733712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5204,11 +5205,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296154368"/>
-        <c:axId val="296153584"/>
+        <c:axId val="431736456"/>
+        <c:axId val="431734888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296154368"/>
+        <c:axId val="431736456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5218,7 +5219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296153584"/>
+        <c:crossAx val="431734888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5226,7 +5227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296153584"/>
+        <c:axId val="431734888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5237,7 +5238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296154368"/>
+        <c:crossAx val="431736456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5394,11 +5395,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296149272"/>
-        <c:axId val="296146920"/>
+        <c:axId val="431736848"/>
+        <c:axId val="431736064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296149272"/>
+        <c:axId val="431736848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5408,7 +5409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296146920"/>
+        <c:crossAx val="431736064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5416,7 +5417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296146920"/>
+        <c:axId val="431736064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5427,7 +5428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296149272"/>
+        <c:crossAx val="431736848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5590,11 +5591,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296149664"/>
-        <c:axId val="297290720"/>
+        <c:axId val="431735672"/>
+        <c:axId val="431730968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296149664"/>
+        <c:axId val="431735672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5604,7 +5605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297290720"/>
+        <c:crossAx val="431730968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5612,7 +5613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297290720"/>
+        <c:axId val="431730968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5623,7 +5624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296149664"/>
+        <c:crossAx val="431735672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5670,7 +5671,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5798,11 +5798,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297291896"/>
-        <c:axId val="297295032"/>
+        <c:axId val="431711368"/>
+        <c:axId val="431716856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297291896"/>
+        <c:axId val="431711368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5812,7 +5812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="297295032"/>
+        <c:crossAx val="431716856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5820,7 +5820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297295032"/>
+        <c:axId val="431716856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5831,14 +5831,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297291896"/>
+        <c:crossAx val="431711368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5971,11 +5970,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="283655232"/>
-        <c:axId val="283660328"/>
+        <c:axId val="319699576"/>
+        <c:axId val="319699968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="283655232"/>
+        <c:axId val="319699576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5985,7 +5984,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283660328"/>
+        <c:crossAx val="319699968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5993,7 +5992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283660328"/>
+        <c:axId val="319699968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6004,7 +6003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283655232"/>
+        <c:crossAx val="319699576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6176,11 +6175,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297295424"/>
-        <c:axId val="297297776"/>
+        <c:axId val="431709800"/>
+        <c:axId val="431707056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297295424"/>
+        <c:axId val="431709800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6190,7 +6189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297297776"/>
+        <c:crossAx val="431707056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6198,7 +6197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297297776"/>
+        <c:axId val="431707056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6209,7 +6208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297295424"/>
+        <c:crossAx val="431709800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6379,11 +6378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297293464"/>
-        <c:axId val="297291112"/>
+        <c:axId val="431710584"/>
+        <c:axId val="431708624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297293464"/>
+        <c:axId val="431710584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6393,7 +6392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297291112"/>
+        <c:crossAx val="431708624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6401,7 +6400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297291112"/>
+        <c:axId val="431708624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6412,7 +6411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297293464"/>
+        <c:crossAx val="431710584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6582,11 +6581,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297291504"/>
-        <c:axId val="297293856"/>
+        <c:axId val="431709016"/>
+        <c:axId val="431714896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297291504"/>
+        <c:axId val="431709016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6596,7 +6595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297293856"/>
+        <c:crossAx val="431714896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6604,7 +6603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297293856"/>
+        <c:axId val="431714896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6615,7 +6614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297291504"/>
+        <c:crossAx val="431709016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6779,11 +6778,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297287584"/>
-        <c:axId val="297292288"/>
+        <c:axId val="431709408"/>
+        <c:axId val="431713328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297287584"/>
+        <c:axId val="431709408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6793,7 +6792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297292288"/>
+        <c:crossAx val="431713328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6801,7 +6800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297292288"/>
+        <c:axId val="431713328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6812,7 +6811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297287584"/>
+        <c:crossAx val="431709408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6982,11 +6981,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297288760"/>
-        <c:axId val="297295816"/>
+        <c:axId val="431711760"/>
+        <c:axId val="431712152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297288760"/>
+        <c:axId val="431711760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6996,7 +6995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297295816"/>
+        <c:crossAx val="431712152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7004,7 +7003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297295816"/>
+        <c:axId val="431712152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7015,7 +7014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297288760"/>
+        <c:crossAx val="431711760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7179,11 +7178,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297290328"/>
-        <c:axId val="297287192"/>
+        <c:axId val="431712544"/>
+        <c:axId val="431712936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297290328"/>
+        <c:axId val="431712544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7193,7 +7192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297287192"/>
+        <c:crossAx val="431712936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7201,7 +7200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297287192"/>
+        <c:axId val="431712936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7212,7 +7211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297290328"/>
+        <c:crossAx val="431712544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7382,11 +7381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297287976"/>
-        <c:axId val="297296208"/>
+        <c:axId val="431714504"/>
+        <c:axId val="431714112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297287976"/>
+        <c:axId val="431714504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7396,7 +7395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297296208"/>
+        <c:crossAx val="431714112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7404,7 +7403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297296208"/>
+        <c:axId val="431714112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7415,7 +7414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297287976"/>
+        <c:crossAx val="431714504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7579,11 +7578,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297289936"/>
-        <c:axId val="297296600"/>
+        <c:axId val="431716072"/>
+        <c:axId val="431716464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297289936"/>
+        <c:axId val="431716072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7593,7 +7592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297296600"/>
+        <c:crossAx val="431716464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7601,7 +7600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297296600"/>
+        <c:axId val="431716464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7612,7 +7611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297289936"/>
+        <c:crossAx val="431716072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7782,11 +7781,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297294640"/>
-        <c:axId val="297296992"/>
+        <c:axId val="431717248"/>
+        <c:axId val="431717640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297294640"/>
+        <c:axId val="431717248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7796,7 +7795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297296992"/>
+        <c:crossAx val="431717640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7804,7 +7803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297296992"/>
+        <c:axId val="431717640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7815,7 +7814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297294640"/>
+        <c:crossAx val="431717248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7979,11 +7978,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297302088"/>
-        <c:axId val="297300912"/>
+        <c:axId val="431706664"/>
+        <c:axId val="431727832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297302088"/>
+        <c:axId val="431706664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7993,7 +7992,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297300912"/>
+        <c:crossAx val="431727832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8001,7 +8000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297300912"/>
+        <c:axId val="431727832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8012,7 +8011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297302088"/>
+        <c:crossAx val="431706664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8167,11 +8166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="283661112"/>
-        <c:axId val="283659544"/>
+        <c:axId val="319703104"/>
+        <c:axId val="319703888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="283661112"/>
+        <c:axId val="319703104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8199,12 +8198,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283659544"/>
+        <c:crossAx val="319703888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="283659544"/>
+        <c:axId val="319703888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8233,7 +8232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283661112"/>
+        <c:crossAx val="319703104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8403,11 +8402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297301696"/>
-        <c:axId val="297298952"/>
+        <c:axId val="431719208"/>
+        <c:axId val="431725088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297301696"/>
+        <c:axId val="431719208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8417,7 +8416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297298952"/>
+        <c:crossAx val="431725088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8425,7 +8424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297298952"/>
+        <c:axId val="431725088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8436,7 +8435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297301696"/>
+        <c:crossAx val="431719208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8600,11 +8599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297299736"/>
-        <c:axId val="297300128"/>
+        <c:axId val="431721952"/>
+        <c:axId val="431721168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297299736"/>
+        <c:axId val="431721952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8614,7 +8613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297300128"/>
+        <c:crossAx val="431721168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8622,7 +8621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297300128"/>
+        <c:axId val="431721168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8633,7 +8632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297299736"/>
+        <c:crossAx val="431721952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8803,11 +8802,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298255128"/>
-        <c:axId val="298257480"/>
+        <c:axId val="431719600"/>
+        <c:axId val="431729008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298255128"/>
+        <c:axId val="431719600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8817,7 +8816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298257480"/>
+        <c:crossAx val="431729008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8825,7 +8824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298257480"/>
+        <c:axId val="431729008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8836,7 +8835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298255128"/>
+        <c:crossAx val="431719600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9000,11 +8999,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298255520"/>
-        <c:axId val="298255912"/>
+        <c:axId val="431719992"/>
+        <c:axId val="431720384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298255520"/>
+        <c:axId val="431719992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9014,7 +9013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298255912"/>
+        <c:crossAx val="431720384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9022,7 +9021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298255912"/>
+        <c:axId val="431720384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9033,7 +9032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298255520"/>
+        <c:crossAx val="431719992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9203,11 +9202,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298257088"/>
-        <c:axId val="298256304"/>
+        <c:axId val="431722344"/>
+        <c:axId val="431722736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298257088"/>
+        <c:axId val="431722344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9217,7 +9216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298256304"/>
+        <c:crossAx val="431722736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9225,7 +9224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298256304"/>
+        <c:axId val="431722736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9236,7 +9235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298257088"/>
+        <c:crossAx val="431722344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9400,11 +9399,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298247680"/>
-        <c:axId val="298246112"/>
+        <c:axId val="431725872"/>
+        <c:axId val="431723912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298247680"/>
+        <c:axId val="431725872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9414,7 +9413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298246112"/>
+        <c:crossAx val="431723912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9422,7 +9421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298246112"/>
+        <c:axId val="431723912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9433,7 +9432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298247680"/>
+        <c:crossAx val="431725872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9603,11 +9602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298249640"/>
-        <c:axId val="298246504"/>
+        <c:axId val="431726264"/>
+        <c:axId val="431726656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298249640"/>
+        <c:axId val="431726264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9617,7 +9616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298246504"/>
+        <c:crossAx val="431726656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9625,7 +9624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298246504"/>
+        <c:axId val="431726656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9636,7 +9635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298249640"/>
+        <c:crossAx val="431726264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9800,11 +9799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298246896"/>
-        <c:axId val="298247288"/>
+        <c:axId val="431718424"/>
+        <c:axId val="431718816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298246896"/>
+        <c:axId val="431718424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9814,7 +9813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298247288"/>
+        <c:crossAx val="431718816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9822,7 +9821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298247288"/>
+        <c:axId val="431718816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9833,7 +9832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298246896"/>
+        <c:crossAx val="431718424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10003,11 +10002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298252776"/>
-        <c:axId val="298244936"/>
+        <c:axId val="431720776"/>
+        <c:axId val="431728224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298252776"/>
+        <c:axId val="431720776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10017,7 +10016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298244936"/>
+        <c:crossAx val="431728224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10025,7 +10024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298244936"/>
+        <c:axId val="431728224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10036,7 +10035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298252776"/>
+        <c:crossAx val="431720776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10200,11 +10199,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298252384"/>
-        <c:axId val="298250032"/>
+        <c:axId val="431729792"/>
+        <c:axId val="431730184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298252384"/>
+        <c:axId val="431729792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10214,7 +10213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298250032"/>
+        <c:crossAx val="431730184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10222,7 +10221,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298250032"/>
+        <c:axId val="431730184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10233,7 +10232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298252384"/>
+        <c:crossAx val="431729792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10387,11 +10386,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="283657192"/>
-        <c:axId val="283657584"/>
+        <c:axId val="319701536"/>
+        <c:axId val="331113816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="283657192"/>
+        <c:axId val="319701536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10419,12 +10418,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283657584"/>
+        <c:crossAx val="331113816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="283657584"/>
+        <c:axId val="331113816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10453,7 +10452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283657192"/>
+        <c:crossAx val="319701536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10617,11 +10616,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298241800"/>
-        <c:axId val="298250816"/>
+        <c:axId val="328630640"/>
+        <c:axId val="328627504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298241800"/>
+        <c:axId val="328630640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10631,7 +10630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298250816"/>
+        <c:crossAx val="328627504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10639,7 +10638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298250816"/>
+        <c:axId val="328627504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10650,7 +10649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298241800"/>
+        <c:crossAx val="328630640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10814,11 +10813,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298242976"/>
-        <c:axId val="298248464"/>
+        <c:axId val="328631816"/>
+        <c:axId val="328632992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298242976"/>
+        <c:axId val="328631816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10828,7 +10827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298248464"/>
+        <c:crossAx val="328632992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10836,7 +10835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298248464"/>
+        <c:axId val="328632992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10847,7 +10846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298242976"/>
+        <c:crossAx val="328631816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11011,11 +11010,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298249248"/>
-        <c:axId val="298251208"/>
+        <c:axId val="328622408"/>
+        <c:axId val="328622800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298249248"/>
+        <c:axId val="328622408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11025,7 +11024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298251208"/>
+        <c:crossAx val="328622800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11033,7 +11032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298251208"/>
+        <c:axId val="328622800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11044,7 +11043,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298249248"/>
+        <c:crossAx val="328622408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11208,11 +11207,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298242192"/>
-        <c:axId val="298242584"/>
+        <c:axId val="328627112"/>
+        <c:axId val="328634560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298242192"/>
+        <c:axId val="328627112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11222,7 +11221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298242584"/>
+        <c:crossAx val="328634560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11230,7 +11229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298242584"/>
+        <c:axId val="328634560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11241,7 +11240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298242192"/>
+        <c:crossAx val="328627112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11399,11 +11398,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298243368"/>
-        <c:axId val="298243760"/>
+        <c:axId val="328623192"/>
+        <c:axId val="328631424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298243368"/>
+        <c:axId val="328623192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11413,7 +11412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298243760"/>
+        <c:crossAx val="328631424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11421,7 +11420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298243760"/>
+        <c:axId val="328631424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11432,7 +11431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298243368"/>
+        <c:crossAx val="328623192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11578,11 +11577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298244544"/>
-        <c:axId val="298245720"/>
+        <c:axId val="328632208"/>
+        <c:axId val="328626720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298244544"/>
+        <c:axId val="328632208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11592,7 +11591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298245720"/>
+        <c:crossAx val="328626720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11600,7 +11599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298245720"/>
+        <c:axId val="328626720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11611,7 +11610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298244544"/>
+        <c:crossAx val="328632208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11763,11 +11762,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298561272"/>
-        <c:axId val="298562448"/>
+        <c:axId val="328632600"/>
+        <c:axId val="328624760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298561272"/>
+        <c:axId val="328632600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11777,7 +11776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298562448"/>
+        <c:crossAx val="328624760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11785,7 +11784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298562448"/>
+        <c:axId val="328624760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11796,7 +11795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298561272"/>
+        <c:crossAx val="328632600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11954,11 +11953,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="298567936"/>
-        <c:axId val="298567152"/>
+        <c:axId val="328627896"/>
+        <c:axId val="328623976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298567936"/>
+        <c:axId val="328627896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11968,7 +11967,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298567152"/>
+        <c:crossAx val="328623976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11976,7 +11975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298567152"/>
+        <c:axId val="328623976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11987,7 +11986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298567936"/>
+        <c:crossAx val="328627896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12044,6 +12043,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12275,11 +12275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="298563624"/>
-        <c:axId val="298566760"/>
+        <c:axId val="328625544"/>
+        <c:axId val="328633384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="298563624"/>
+        <c:axId val="328625544"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12339,12 +12339,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298566760"/>
+        <c:crossAx val="328633384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="298566760"/>
+        <c:axId val="328633384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12403,7 +12403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298563624"/>
+        <c:crossAx val="328625544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12557,8 +12557,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="298564016"/>
-        <c:axId val="298565192"/>
+        <c:axId val="328624368"/>
+        <c:axId val="328625936"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12712,11 +12712,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="298564016"/>
-        <c:axId val="298565192"/>
+        <c:axId val="328624368"/>
+        <c:axId val="328625936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298564016"/>
+        <c:axId val="328624368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12726,7 +12726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298565192"/>
+        <c:crossAx val="328625936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12734,7 +12734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298565192"/>
+        <c:axId val="328625936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12745,13 +12745,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298564016"/>
+        <c:crossAx val="328624368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12947,11 +12948,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="283658368"/>
-        <c:axId val="283659152"/>
+        <c:axId val="331119696"/>
+        <c:axId val="331118128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="283658368"/>
+        <c:axId val="331119696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12961,7 +12962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283659152"/>
+        <c:crossAx val="331118128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12969,7 +12970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283659152"/>
+        <c:axId val="331118128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12980,7 +12981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="283658368"/>
+        <c:crossAx val="331119696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13084,8 +13085,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="298564800"/>
-        <c:axId val="298567544"/>
+        <c:axId val="328631032"/>
+        <c:axId val="328634168"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13203,11 +13204,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="298564800"/>
-        <c:axId val="298567544"/>
+        <c:axId val="328631032"/>
+        <c:axId val="328634168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298564800"/>
+        <c:axId val="328631032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13217,7 +13218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298567544"/>
+        <c:crossAx val="328634168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13225,7 +13226,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298567544"/>
+        <c:axId val="328634168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13236,7 +13237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298564800"/>
+        <c:crossAx val="328631032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13404,11 +13405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296258664"/>
-        <c:axId val="296260232"/>
+        <c:axId val="331116168"/>
+        <c:axId val="331114208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296258664"/>
+        <c:axId val="331116168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13418,7 +13419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296260232"/>
+        <c:crossAx val="331114208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13426,7 +13427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296260232"/>
+        <c:axId val="331114208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13437,7 +13438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296258664"/>
+        <c:crossAx val="331116168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13601,11 +13602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296261016"/>
-        <c:axId val="296259840"/>
+        <c:axId val="331118912"/>
+        <c:axId val="331115384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296261016"/>
+        <c:axId val="331118912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13615,7 +13616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296259840"/>
+        <c:crossAx val="331115384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13623,7 +13624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296259840"/>
+        <c:axId val="331115384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13634,7 +13635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296261016"/>
+        <c:crossAx val="331118912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13798,11 +13799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296263368"/>
-        <c:axId val="296262192"/>
+        <c:axId val="331114992"/>
+        <c:axId val="331116952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296263368"/>
+        <c:axId val="331114992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13812,7 +13813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296262192"/>
+        <c:crossAx val="331116952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13820,7 +13821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296262192"/>
+        <c:axId val="331116952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13831,7 +13832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296263368"/>
+        <c:crossAx val="331114992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17228,6 +17229,678 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3">
+        <v>40921</v>
+      </c>
+      <c r="D2">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>0-C5</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>H5/10000</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J15" si="0">D5*I5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2.25</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>0.02</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E15" si="1">0-C6</f>
+        <v>-26</v>
+      </c>
+      <c r="F6">
+        <f>(B6-B5)*12</f>
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <f>F6*2.54</f>
+        <v>68.58</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H15" si="2">G6*((C6+C5)/2)</f>
+        <v>891.54</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I15" si="3">H6/10000</f>
+        <v>8.9153999999999997E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1.78308E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2.5</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>0.03</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-24</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F15" si="4">(B7-B6)*12</f>
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G20" si="5">F7*2.54</f>
+        <v>7.62</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>190.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>1.9050000000000001E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>5.7149999999999996E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>0.04</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>-31</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>419.1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>4.1910000000000003E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1.6764000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>3.5</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>0.02</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-26</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>434.34000000000003</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>4.3434E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>8.6868000000000004E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>0.02</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>-29</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>419.1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>4.1910000000000003E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>8.382000000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>4.5</v>
+      </c>
+      <c r="C11">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>0.01</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-29</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>441.96</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>4.4195999999999999E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>4.4195999999999998E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>0.02</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>-27</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>426.72</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>4.2672000000000002E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>8.5344000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5.5</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>0.03</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-24</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>388.62</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>3.8862000000000001E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1.1658599999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>0.01</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>-21</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>342.9</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>3.4290000000000001E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>3.4290000000000004E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6.5</v>
+      </c>
+      <c r="C15">
+        <v>26.5</v>
+      </c>
+      <c r="D15">
+        <v>0.01</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>-26.5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>361.95</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>3.6194999999999998E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>3.6194999999999999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>0.01</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E20" si="6">0-C16</f>
+        <v>-16</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F20" si="7">(B16-B15)*12</f>
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H20" si="8">G16*((C16+C15)/2)</f>
+        <v>323.85000000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I20" si="9">H16/10000</f>
+        <v>3.2385000000000004E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J20" si="10">D16*I16</f>
+        <v>3.2385000000000004E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7.5</v>
+      </c>
+      <c r="C17">
+        <v>20.5</v>
+      </c>
+      <c r="D17">
+        <v>0.01</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>-20.5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="8"/>
+        <v>278.13</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="9"/>
+        <v>2.7813000000000001E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="10"/>
+        <v>2.7813000000000002E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>0.01</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>-18</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="8"/>
+        <v>293.37</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="9"/>
+        <v>2.9337000000000002E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="10"/>
+        <v>2.9337000000000005E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8.5</v>
+      </c>
+      <c r="C19">
+        <v>18.5</v>
+      </c>
+      <c r="D19">
+        <v>0.02</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>-18.5</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>15.24</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="8"/>
+        <v>278.13</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>2.7813000000000001E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="10"/>
+        <v>5.5626000000000004E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>8.75</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>7.62</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="8"/>
+        <v>70.484999999999999</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="9"/>
+        <v>7.0485000000000001E-3</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <f>SUM(J5:J15)</f>
+        <v>8.9039699999999989E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <f>J21*1000</f>
+        <v>8.9039699999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17685,7 +18358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J14"/>
   <sheetViews>
@@ -18074,7 +18747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J15"/>
   <sheetViews>
@@ -18498,7 +19171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J17"/>
   <sheetViews>
@@ -18986,15 +19659,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O41" sqref="O41"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21360,7 +22033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R9"/>
   <sheetViews>
@@ -21630,7 +22303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J27"/>
   <sheetViews>
@@ -22145,7 +22818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S81"/>
   <sheetViews>
@@ -24186,7 +24859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S77"/>
   <sheetViews>
@@ -40694,7 +41367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D320" workbookViewId="0">
+    <sheetView topLeftCell="D320" workbookViewId="0">
       <selection activeCell="E335" sqref="E335:G351"/>
     </sheetView>
   </sheetViews>
@@ -47710,6 +48383,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
@@ -48256,7 +48941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J17"/>
   <sheetViews>
@@ -48753,7 +49438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J18"/>
   <sheetViews>
@@ -49286,7 +49971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J17"/>
   <sheetViews>
@@ -49781,676 +50466,4 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3">
-        <v>40921</v>
-      </c>
-      <c r="D2">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>0-C5</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>H5/10000</f>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J15" si="0">D5*I5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2.25</v>
-      </c>
-      <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>0.02</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E15" si="1">0-C6</f>
-        <v>-26</v>
-      </c>
-      <c r="F6">
-        <f>(B6-B5)*12</f>
-        <v>27</v>
-      </c>
-      <c r="G6">
-        <f>F6*2.54</f>
-        <v>68.58</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H15" si="2">G6*((C6+C5)/2)</f>
-        <v>891.54</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I15" si="3">H6/10000</f>
-        <v>8.9153999999999997E-2</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.78308E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>2.5</v>
-      </c>
-      <c r="C7">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>0.03</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>-24</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F15" si="4">(B7-B6)*12</f>
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ref="G7:G20" si="5">F7*2.54</f>
-        <v>7.62</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>190.5</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
-        <v>1.9050000000000001E-2</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>5.7149999999999996E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>31</v>
-      </c>
-      <c r="D8">
-        <v>0.04</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>-31</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>419.1</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="3"/>
-        <v>4.1910000000000003E-2</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1.6764000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
-        <v>3.5</v>
-      </c>
-      <c r="C9">
-        <v>26</v>
-      </c>
-      <c r="D9">
-        <v>0.02</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>-26</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>434.34000000000003</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>4.3434E-2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>8.6868000000000004E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <v>0.02</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>-29</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>419.1</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="3"/>
-        <v>4.1910000000000003E-2</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>8.382000000000001E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>4.5</v>
-      </c>
-      <c r="C11">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>0.01</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>-29</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>441.96</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>4.4195999999999999E-2</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>4.4195999999999998E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>27</v>
-      </c>
-      <c r="D12">
-        <v>0.02</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>-27</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>426.72</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="3"/>
-        <v>4.2672000000000002E-2</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>8.5344000000000001E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>5.5</v>
-      </c>
-      <c r="C13">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>0.03</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>-24</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>388.62</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
-        <v>3.8862000000000001E-2</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>1.1658599999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>21</v>
-      </c>
-      <c r="D14">
-        <v>0.01</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>-21</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>342.9</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
-        <v>3.4290000000000001E-2</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>3.4290000000000004E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>6.5</v>
-      </c>
-      <c r="C15">
-        <v>26.5</v>
-      </c>
-      <c r="D15">
-        <v>0.01</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>-26.5</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>361.95</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
-        <v>3.6194999999999998E-2</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>3.6194999999999999E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>16</v>
-      </c>
-      <c r="D16">
-        <v>0.01</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ref="E16:E20" si="6">0-C16</f>
-        <v>-16</v>
-      </c>
-      <c r="F16">
-        <f t="shared" ref="F16:F20" si="7">(B16-B15)*12</f>
-        <v>6</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ref="H16:H20" si="8">G16*((C16+C15)/2)</f>
-        <v>323.85000000000002</v>
-      </c>
-      <c r="I16">
-        <f t="shared" ref="I16:I20" si="9">H16/10000</f>
-        <v>3.2385000000000004E-2</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ref="J16:J20" si="10">D16*I16</f>
-        <v>3.2385000000000004E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>7.5</v>
-      </c>
-      <c r="C17">
-        <v>20.5</v>
-      </c>
-      <c r="D17">
-        <v>0.01</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="6"/>
-        <v>-20.5</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="8"/>
-        <v>278.13</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="9"/>
-        <v>2.7813000000000001E-2</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="10"/>
-        <v>2.7813000000000002E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>0.01</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="6"/>
-        <v>-18</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="8"/>
-        <v>293.37</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="9"/>
-        <v>2.9337000000000002E-2</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="10"/>
-        <v>2.9337000000000005E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>8.5</v>
-      </c>
-      <c r="C19">
-        <v>18.5</v>
-      </c>
-      <c r="D19">
-        <v>0.02</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="6"/>
-        <v>-18.5</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>15.24</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="8"/>
-        <v>278.13</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="9"/>
-        <v>2.7813000000000001E-2</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="10"/>
-        <v>5.5626000000000004E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>8.75</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="5"/>
-        <v>7.62</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="8"/>
-        <v>70.484999999999999</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="9"/>
-        <v>7.0485000000000001E-3</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21">
-        <f>SUM(J5:J15)</f>
-        <v>8.9039699999999989E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22">
-        <f>J21*1000</f>
-        <v>8.9039699999999993</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>